<commit_message>
Fixed Threading Issue,Need ExcelCombine to work properly
</commit_message>
<xml_diff>
--- a/kayakPrices.xlsx
+++ b/kayakPrices.xlsx
@@ -14,162 +14,192 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="52">
-  <si>
-    <t>8:40 pm–11:25 pm</t>
-  </si>
-  <si>
-    <t>6:05 am–8:55 am</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="62">
+  <si>
+    <t>9:00 am–11:05 am</t>
+  </si>
+  <si>
+    <t>6:00 pm–8:00 pm</t>
   </si>
   <si>
     <t>Economy</t>
   </si>
   <si>
-    <t>www.kayak.com/book/flight?code=PfGiC4BdBS.18wgSzIaLAlgpzrTH2pViLaYAeeTFjgE.41297.ee53b680731d1284e16f78c26827d777&amp;h=4e0944041bbc&amp;sub=E-13704b0953d&amp;pageOrigin=F..RP.FE.M1</t>
+    <t>www.kayak.com/s/clickthrough.jsp?ctyp=SponsoredResultAdBooking&amp;ptyp=F&amp;orig=F..RP..M1&amp;plid=5246637&amp;pid=eDreams_FSR_US&amp;prv=eDreams_FSR_US&amp;srch=PiGCFO1ZAy&amp;ploc=US&amp;atype=SponsoredResult&amp;prc=131.00&amp;cpnid=5011374&amp;xpExt=&amp;aidExt=&amp;lid=eDreams_FSR_US-PiGCFO1ZAy&amp;qorig=Airport:DEL&amp;octid=&amp;qdest=Airport:BOM&amp;qstart=1684382400000&amp;qend=1684987200000&amp;qtravelers=1&amp;qrooms=0&amp;qow=false&amp;qfcc=e&amp;qdctid=31288&amp;qdac=BOM&amp;qshour=-1&amp;qehour=-1&amp;qns=false&amp;qnearby=0&amp;qnearbyo=false&amp;qnearbyd=false&amp;pj=y$2pw5mvU8arrrIA6kFdxw==&amp;ah=MXefH5bqhl7nYyTMeopoSqCW4YP_RM4Pcf3vX4qXV$Q&amp;resid=503e6d46c0f023f9f47ed4bf3e9bf5c4&amp;bookid=E-1ea59fda05f&amp;seekProv=EDREAMSAIR&amp;trueProv=EDREAMSAIR&amp;fid=&amp;rank=1&amp;stid=&amp;qadults=1&amp;qchild=0&amp;_sid_=R-53lYaBnvdpR1xqacnhy1A-Kbs0GBHnbsYQzZz9_CgW1decfCM3HwBeADA0IdtMT&amp;pageOrigin=F..RP.FE.M0</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>6:20 pm–9:10 pm</t>
-  </si>
-  <si>
-    <t>www.kayak.com/book/flight?code=PfGiC4BdBS.vCxqPNdeNfxFj024N3_sTg.53533.843ba14281c3d147b11e9b46909cedee&amp;h=896c9a54650a&amp;sub=E-140dc59a55d&amp;pageOrigin=F..RP.FE.M2</t>
-  </si>
-  <si>
-    <t>11:00 pm–10:45 am+1</t>
-  </si>
-  <si>
-    <t>10:00 am–4:15 am+1</t>
-  </si>
-  <si>
-    <t>www.kayak.com/book/flight?code=PfGiC4BdBS.4Gcos1vZgwmejng0G6qX_yzU0H9G2WiK.61994.a52be6545fe10be86dbb160fa797b506&amp;h=9fb042a3d7b8&amp;sub=E-17545a7e6a1&amp;pageOrigin=F..RP.FE.M4</t>
-  </si>
-  <si>
-    <t>12:15 pm–6:35 pm</t>
-  </si>
-  <si>
-    <t>2:20 pm–4:40 pm+1</t>
-  </si>
-  <si>
-    <t>www.kayak.com/book/flight?code=PfGiC4BdBS.vCxqPNdeNfxFj024N3_sTg.93542.9b3361b504ac19827ff759f3f27ed462&amp;h=b798275ef14f&amp;sub=E-140dc59a55d&amp;pageOrigin=F..RP.FE.M5</t>
-  </si>
-  <si>
-    <t>8:00 pm–8:00 am+1</t>
-  </si>
-  <si>
-    <t>7:25 pm–10:35 pm+1</t>
-  </si>
-  <si>
-    <t>www.kayak.com/book/flight?code=PfGiC4BdBS.vCxqPNdeNfxFj024N3_sTg.88958.a7b7ba533f23d925e3f7ad1e649c94e1&amp;h=3d4170c395d6&amp;sub=E-140dc59a55d&amp;pageOrigin=F..RP.FE.M7</t>
-  </si>
-  <si>
-    <t>11:30 pm–12:01 am+2</t>
-  </si>
-  <si>
-    <t>www.kayak.com/book/flight?code=PfGiC4BdBS.4Gcos1vZgwmejng0G6qX_yzU0H9G2WiK.80964.b826144f0cc916bf5cc269eced4aee38&amp;h=672c33e8971a&amp;sub=E-17545a7e6a1&amp;pageOrigin=F..RP.FE.M8</t>
+    <t>7:00 am–9:15 am</t>
+  </si>
+  <si>
+    <t>6:15 pm–8:15 pm</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13000.e7d8a05ac45b309f0894385a59df86a4&amp;h=890f6545ec17&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M1</t>
+  </si>
+  <si>
+    <t>5:00 am–11:25 am</t>
+  </si>
+  <si>
+    <t>2:45 pm–10:45 pm</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.JZO1f6NT9B8-ciubBqDvug.10846.30658953724d5cbc585ec5cc369c43ca&amp;h=761eee518e43&amp;sub=E-1fb91230d28&amp;pageOrigin=F..RP.FE.M2</t>
+  </si>
+  <si>
+    <t>8:00 am–10:20 am</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13000.66c2c907ec0a7812876f8be6b77bd32e&amp;h=755b01757c2f&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M5</t>
+  </si>
+  <si>
+    <t>9:00 am–11:20 am</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13000.4778d696526d298e31dda4f13a36ca71&amp;h=8234409ef6ca&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M6</t>
+  </si>
+  <si>
+    <t>2:00 pm–4:20 pm</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13000.b15032367203c5cdd574b6d647941d68&amp;h=9ecbf4262e63&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M7</t>
+  </si>
+  <si>
+    <t>8:00 pm–10:10 pm</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13800.97f8fbc73c9bc93bd8296e61633e93d4&amp;h=aa8d5cee5d08&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M9</t>
+  </si>
+  <si>
+    <t>10:00 am–12:30 pm</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13000.77526e730915bc57bcf19ba488c685c0&amp;h=774c14703de5&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M10</t>
+  </si>
+  <si>
+    <t>8:00 am–10:15 am</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13000.bd1dfa71bf8a59ecf84ef8522955d5bb&amp;h=2b93c7af0c91&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M11</t>
+  </si>
+  <si>
+    <t>1:00 pm–3:15 pm</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13000.7b26c33cb5e6a161429aac5e4b42958e&amp;h=866d296683bf&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M12</t>
+  </si>
+  <si>
+    <t>7:00 pm–9:15 pm</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13000.0199eb315decba4c133dfd4cde6eb9a6&amp;h=29669fd4c39f&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M13</t>
+  </si>
+  <si>
+    <t>5:40 pm–8:10 pm</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13000.5e912bc9f64ff152d3a9daed993e4d7b&amp;h=1dece8b328b5&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M14</t>
+  </si>
+  <si>
+    <t>6:00 am–8:00 am</t>
+  </si>
+  <si>
+    <t>11:55 am–1:55 pm</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.UwQrSnW3-tbTYwQ_VUUUMA.15100.e1bf42b28a2e3a5b7497af61ca39002f&amp;h=2d99b523dad6&amp;sub=E-16a352879f0&amp;pageOrigin=F..RP.FE.M15</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.15100.d9d37383db5f3c05f17da900a662f93c&amp;h=f13cf457fd7b&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M17</t>
+  </si>
+  <si>
+    <t>9:30 am–11:35 am</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.15000.a0fc6092174046348d7d38cdb80c70eb&amp;h=f21f938add2b&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M18</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13000.e5b4e2394ab8aaf774f70e141d260a37&amp;h=5e19886a0b79&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M19</t>
+  </si>
+  <si>
+    <t>www.kayak.com/book/flight?code=PiGCFO1ZAy.mgYptEKS7RsDzQq2dWkU9A.13000.151b63390e79935c6695cedad3d7a06d&amp;h=2bd8ede5fc80&amp;sub=E-117dccc01c7&amp;pageOrigin=F..RP.FE.M20</t>
   </si>
   <si>
     <t>IndiGo</t>
   </si>
   <si>
-    <t>SpiceJet</t>
-  </si>
-  <si>
-    <t>Alaska Seaplanes</t>
-  </si>
-  <si>
-    <t>Malaysia Airlines</t>
-  </si>
-  <si>
-    <t>SriLankan Airlines</t>
-  </si>
-  <si>
-    <t>Alaska Seaplanes, SpiceJet</t>
-  </si>
-  <si>
-    <t>SpiceJet, Alaska Seaplanes</t>
-  </si>
-  <si>
-    <t>Thai Airways</t>
-  </si>
-  <si>
-    <t>KUL</t>
-  </si>
-  <si>
-    <t>CMB</t>
-  </si>
-  <si>
-    <t>SAG</t>
+    <t>Air India</t>
+  </si>
+  <si>
+    <t>AirAsia India</t>
+  </si>
+  <si>
+    <t>Vistara</t>
+  </si>
+  <si>
+    <t>JAI</t>
+  </si>
+  <si>
+    <t>DEL-BOM</t>
+  </si>
+  <si>
+    <t>BOM-DEL</t>
+  </si>
+  <si>
+    <t>DEL</t>
   </si>
   <si>
     <t>BOM</t>
   </si>
   <si>
-    <t>BKK</t>
-  </si>
-  <si>
-    <t>DEL-MAA</t>
-  </si>
-  <si>
-    <t>MAA-DEL</t>
-  </si>
-  <si>
-    <t>DEL</t>
-  </si>
-  <si>
-    <t>MAA</t>
-  </si>
-  <si>
     <t>nonstop</t>
   </si>
   <si>
     <t>1 stop</t>
   </si>
   <si>
-    <t>2h 45m</t>
-  </si>
-  <si>
-    <t>2h 50m</t>
-  </si>
-  <si>
-    <t>11h 45m</t>
-  </si>
-  <si>
-    <t>18h 15m</t>
-  </si>
-  <si>
-    <t>6h 20m</t>
-  </si>
-  <si>
-    <t>26h 20m</t>
-  </si>
-  <si>
-    <t>12h 00m</t>
-  </si>
-  <si>
-    <t>27h 10m</t>
-  </si>
-  <si>
-    <t>24h 31m</t>
-  </si>
-  <si>
-    <t>$413</t>
-  </si>
-  <si>
-    <t>$536</t>
-  </si>
-  <si>
-    <t>$620</t>
-  </si>
-  <si>
-    <t>$936</t>
-  </si>
-  <si>
-    <t>$890</t>
-  </si>
-  <si>
-    <t>$810</t>
+    <t>2h 05m</t>
+  </si>
+  <si>
+    <t>2h 00m</t>
+  </si>
+  <si>
+    <t>2h 15m</t>
+  </si>
+  <si>
+    <t>6h 25m</t>
+  </si>
+  <si>
+    <t>8h 00m</t>
+  </si>
+  <si>
+    <t>2h 20m</t>
+  </si>
+  <si>
+    <t>2h 10m</t>
+  </si>
+  <si>
+    <t>2h 30m</t>
+  </si>
+  <si>
+    <t>$131</t>
+  </si>
+  <si>
+    <t>$130</t>
+  </si>
+  <si>
+    <t>$109</t>
+  </si>
+  <si>
+    <t>$138</t>
+  </si>
+  <si>
+    <t>$151</t>
+  </si>
+  <si>
+    <t>$150</t>
   </si>
 </sst>
 </file>
@@ -527,7 +557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -567,22 +597,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -590,25 +620,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -631,48 +661,48 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -682,7 +712,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -692,57 +722,57 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="I13" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -752,7 +782,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -762,57 +792,51 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G17" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H17" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H18" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="I18" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -835,54 +859,48 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G22" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H22" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H23" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I23" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -892,7 +910,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -902,57 +920,51 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G27" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H27" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F28" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G28" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="H28" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="I28" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -962,11 +974,715 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" t="s">
+        <v>49</v>
+      </c>
+      <c r="I33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" t="s">
+        <v>46</v>
+      </c>
+      <c r="H38" t="s">
+        <v>49</v>
+      </c>
+      <c r="I38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s">
+        <v>45</v>
+      </c>
+      <c r="G42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
+        <v>44</v>
+      </c>
+      <c r="G43" t="s">
+        <v>46</v>
+      </c>
+      <c r="H43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" t="s">
+        <v>46</v>
+      </c>
+      <c r="H47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G48" t="s">
+        <v>46</v>
+      </c>
+      <c r="H48" t="s">
+        <v>50</v>
+      </c>
+      <c r="I48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" t="s">
+        <v>46</v>
+      </c>
+      <c r="H52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53" t="s">
+        <v>45</v>
+      </c>
+      <c r="F53" t="s">
+        <v>44</v>
+      </c>
+      <c r="G53" t="s">
+        <v>46</v>
+      </c>
+      <c r="H53" t="s">
+        <v>50</v>
+      </c>
+      <c r="I53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" t="s">
+        <v>42</v>
+      </c>
+      <c r="E57" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" t="s">
+        <v>45</v>
+      </c>
+      <c r="G57" t="s">
+        <v>46</v>
+      </c>
+      <c r="H57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58" t="s">
+        <v>45</v>
+      </c>
+      <c r="F58" t="s">
+        <v>44</v>
+      </c>
+      <c r="G58" t="s">
+        <v>46</v>
+      </c>
+      <c r="H58" t="s">
+        <v>49</v>
+      </c>
+      <c r="I58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>29</v>
+      </c>
+      <c r="B62" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" t="s">
+        <v>42</v>
+      </c>
+      <c r="E62" t="s">
+        <v>44</v>
+      </c>
+      <c r="F62" t="s">
+        <v>45</v>
+      </c>
+      <c r="G62" t="s">
+        <v>46</v>
+      </c>
+      <c r="H62" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63" t="s">
+        <v>40</v>
+      </c>
+      <c r="D63" t="s">
+        <v>43</v>
+      </c>
+      <c r="E63" t="s">
+        <v>45</v>
+      </c>
+      <c r="F63" t="s">
+        <v>44</v>
+      </c>
+      <c r="G63" t="s">
+        <v>46</v>
+      </c>
+      <c r="H63" t="s">
+        <v>49</v>
+      </c>
+      <c r="I63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67" t="s">
+        <v>42</v>
+      </c>
+      <c r="E67" t="s">
+        <v>44</v>
+      </c>
+      <c r="F67" t="s">
+        <v>45</v>
+      </c>
+      <c r="G67" t="s">
+        <v>46</v>
+      </c>
+      <c r="H67" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" t="s">
+        <v>43</v>
+      </c>
+      <c r="E68" t="s">
+        <v>45</v>
+      </c>
+      <c r="F68" t="s">
+        <v>44</v>
+      </c>
+      <c r="G68" t="s">
+        <v>46</v>
+      </c>
+      <c r="H68" t="s">
+        <v>49</v>
+      </c>
+      <c r="I68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>33</v>
+      </c>
+      <c r="B72" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72" t="s">
+        <v>42</v>
+      </c>
+      <c r="E72" t="s">
+        <v>44</v>
+      </c>
+      <c r="F72" t="s">
+        <v>45</v>
+      </c>
+      <c r="G72" t="s">
+        <v>46</v>
+      </c>
+      <c r="H72" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>38</v>
+      </c>
+      <c r="D73" t="s">
+        <v>43</v>
+      </c>
+      <c r="E73" t="s">
+        <v>45</v>
+      </c>
+      <c r="F73" t="s">
+        <v>44</v>
+      </c>
+      <c r="G73" t="s">
+        <v>46</v>
+      </c>
+      <c r="H73" t="s">
+        <v>49</v>
+      </c>
+      <c r="I73" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>11</v>
+      </c>
+      <c r="B77" t="s">
+        <v>38</v>
+      </c>
+      <c r="D77" t="s">
+        <v>42</v>
+      </c>
+      <c r="E77" t="s">
+        <v>44</v>
+      </c>
+      <c r="F77" t="s">
+        <v>45</v>
+      </c>
+      <c r="G77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H77" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>25</v>
+      </c>
+      <c r="B78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D78" t="s">
+        <v>43</v>
+      </c>
+      <c r="E78" t="s">
+        <v>45</v>
+      </c>
+      <c r="F78" t="s">
+        <v>44</v>
+      </c>
+      <c r="G78" t="s">
+        <v>46</v>
+      </c>
+      <c r="H78" t="s">
+        <v>50</v>
+      </c>
+      <c r="I78" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" t="s">
+        <v>11</v>
+      </c>
+      <c r="B82" t="s">
+        <v>38</v>
+      </c>
+      <c r="D82" t="s">
+        <v>42</v>
+      </c>
+      <c r="E82" t="s">
+        <v>44</v>
+      </c>
+      <c r="F82" t="s">
+        <v>45</v>
+      </c>
+      <c r="G82" t="s">
+        <v>46</v>
+      </c>
+      <c r="H82" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" t="s">
+        <v>38</v>
+      </c>
+      <c r="D83" t="s">
+        <v>43</v>
+      </c>
+      <c r="E83" t="s">
+        <v>45</v>
+      </c>
+      <c r="F83" t="s">
+        <v>44</v>
+      </c>
+      <c r="G83" t="s">
+        <v>46</v>
+      </c>
+      <c r="H83" t="s">
+        <v>50</v>
+      </c>
+      <c r="I83" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>